<commit_message>
update all plots with PdeltaAIC included as a covariate for CG also
</commit_message>
<xml_diff>
--- a/tables/CG_PhenT_GenTime.xlsx
+++ b/tables/CG_PhenT_GenTime.xlsx
@@ -41,10 +41,10 @@
     <t xml:space="preserve">0.057</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.574</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1154</t>
+    <t xml:space="preserve">-1.575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1153</t>
   </si>
   <si>
     <t xml:space="preserve">GenLength_y_IUCN.y</t>

</xml_diff>